<commit_message>
change initial data (add emails column)
</commit_message>
<xml_diff>
--- a/mts_hahaton/searcher/file.xlsx
+++ b/mts_hahaton/searcher/file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gavri\Programming\MTS-Hahaton\mts_hahaton\searcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A21DD28-1BD8-4E4E-A94F-EEBE1625701D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3F6608-D039-4709-88D4-9DDD7B13FBD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2016" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2230" uniqueCount="652">
   <si>
     <t xml:space="preserve">Подразделение 1 </t>
   </si>
@@ -1334,6 +1334,648 @@
   </si>
   <si>
     <t>Зайцева</t>
+  </si>
+  <si>
+    <t>xutor-asaza51@mail.ru</t>
+  </si>
+  <si>
+    <t>xadazud_iya10@yandex.ru</t>
+  </si>
+  <si>
+    <t>bemabi-bivi32@list.ru</t>
+  </si>
+  <si>
+    <t>dok-akafike82@bk.ru</t>
+  </si>
+  <si>
+    <t>yeley_ibole71@internet.ru</t>
+  </si>
+  <si>
+    <t>gitihib_ajo54@inbox.ru</t>
+  </si>
+  <si>
+    <t>zeripa-wuvu10@inbox.ru</t>
+  </si>
+  <si>
+    <t>nobate-ziwu33@yahoo.com</t>
+  </si>
+  <si>
+    <t>tivoy_anipi44@list.ru</t>
+  </si>
+  <si>
+    <t>cuto-devivu58@bk.ru</t>
+  </si>
+  <si>
+    <t>rev_efiwimi95@aol.com</t>
+  </si>
+  <si>
+    <t>jeye_sabica11@internet.ru</t>
+  </si>
+  <si>
+    <t>xokecav_ibi37@internet.ru</t>
+  </si>
+  <si>
+    <t>poba-sivife5@inbox.ru</t>
+  </si>
+  <si>
+    <t>fit-ematumi48@yahoo.com</t>
+  </si>
+  <si>
+    <t>lufat_izowi94@list.ru</t>
+  </si>
+  <si>
+    <t>tomorij-izo54@inbox.ru</t>
+  </si>
+  <si>
+    <t>lera_podifu67@inbox.ru</t>
+  </si>
+  <si>
+    <t>wil_ovufete57@internet.ru</t>
+  </si>
+  <si>
+    <t>rugabix-ovo2@bk.ru</t>
+  </si>
+  <si>
+    <t>seyapo_heso31@internet.ru</t>
+  </si>
+  <si>
+    <t>zuzut-obabi30@list.ru</t>
+  </si>
+  <si>
+    <t>log_axayika94@hotmail.com</t>
+  </si>
+  <si>
+    <t>cehi_napipu16@aol.com</t>
+  </si>
+  <si>
+    <t>ximex_ucede30@inbox.ru</t>
+  </si>
+  <si>
+    <t>xobe-pufaxa91@bk.ru</t>
+  </si>
+  <si>
+    <t>hapi_kojeco67@bk.ru</t>
+  </si>
+  <si>
+    <t>tezij_ewizu38@bk.ru</t>
+  </si>
+  <si>
+    <t>migateg_ido82@list.ru</t>
+  </si>
+  <si>
+    <t>givu_mafupu29@aol.com</t>
+  </si>
+  <si>
+    <t>jaya-sokiwi95@internet.ru</t>
+  </si>
+  <si>
+    <t>surosik_aho74@yahoo.com</t>
+  </si>
+  <si>
+    <t>vipoxe-xaza12@mail.ru</t>
+  </si>
+  <si>
+    <t>xiw-amopaca63@gmail.com</t>
+  </si>
+  <si>
+    <t>sobov-etole92@hotmail.com</t>
+  </si>
+  <si>
+    <t>tivawar_oni61@list.ru</t>
+  </si>
+  <si>
+    <t>nif-onaxazu91@bk.ru</t>
+  </si>
+  <si>
+    <t>jovem-egixo30@list.ru</t>
+  </si>
+  <si>
+    <t>podexi-lemu64@mail.ru</t>
+  </si>
+  <si>
+    <t>woran_ehude73@yandex.ru</t>
+  </si>
+  <si>
+    <t>xuba-licace70@bk.ru</t>
+  </si>
+  <si>
+    <t>bifub_ohoti14@yahoo.com</t>
+  </si>
+  <si>
+    <t>sako-takusi31@gmail.com</t>
+  </si>
+  <si>
+    <t>fim-atobome5@hotmail.com</t>
+  </si>
+  <si>
+    <t>nufu_riboje96@bk.ru</t>
+  </si>
+  <si>
+    <t>tolekoh-uji33@list.ru</t>
+  </si>
+  <si>
+    <t>lar_ikibide92@bk.ru</t>
+  </si>
+  <si>
+    <t>tihej_uwawa10@yandex.ru</t>
+  </si>
+  <si>
+    <t>mij_ovokamu25@hotmail.com</t>
+  </si>
+  <si>
+    <t>pixevu_yusu1@yandex.ru</t>
+  </si>
+  <si>
+    <t>buc-ewituho76@internet.ru</t>
+  </si>
+  <si>
+    <t>lipuvi-daro42@gmail.com</t>
+  </si>
+  <si>
+    <t>pux_urikaxa94@bk.ru</t>
+  </si>
+  <si>
+    <t>losanor-ufo20@gmail.com</t>
+  </si>
+  <si>
+    <t>barinic-avo14@bk.ru</t>
+  </si>
+  <si>
+    <t>mapiga-pawo71@gmail.com</t>
+  </si>
+  <si>
+    <t>roxemub-uye95@yandex.ru</t>
+  </si>
+  <si>
+    <t>paxoc_ugaji4@yahoo.com</t>
+  </si>
+  <si>
+    <t>fezu_xuyape35@mail.ru</t>
+  </si>
+  <si>
+    <t>vubon_ijuxi47@yahoo.com</t>
+  </si>
+  <si>
+    <t>vomul_adojo77@internet.ru</t>
+  </si>
+  <si>
+    <t>huhuruv-iyu45@hotmail.com</t>
+  </si>
+  <si>
+    <t>wagad_igama10@hotmail.com</t>
+  </si>
+  <si>
+    <t>goro-vokane46@mail.ru</t>
+  </si>
+  <si>
+    <t>muya_bufome67@inbox.ru</t>
+  </si>
+  <si>
+    <t>puxu_visexu63@aol.com</t>
+  </si>
+  <si>
+    <t>val-enudoye26@gmail.com</t>
+  </si>
+  <si>
+    <t>lurolak_ehe86@yahoo.com</t>
+  </si>
+  <si>
+    <t>sowu_gozeti48@mail.ru</t>
+  </si>
+  <si>
+    <t>hohu_jozice15@list.ru</t>
+  </si>
+  <si>
+    <t>dun_ujelobi3@internet.ru</t>
+  </si>
+  <si>
+    <t>xunocah_uho51@inbox.ru</t>
+  </si>
+  <si>
+    <t>sobovu-tevi49@inbox.ru</t>
+  </si>
+  <si>
+    <t>dedidap-ike57@inbox.ru</t>
+  </si>
+  <si>
+    <t>cogubez-epe45@gmail.com</t>
+  </si>
+  <si>
+    <t>jasak_erefu48@gmail.com</t>
+  </si>
+  <si>
+    <t>zida_puboxa51@mail.ru</t>
+  </si>
+  <si>
+    <t>puy_uhuxaha36@mail.ru</t>
+  </si>
+  <si>
+    <t>daloza-weje61@bk.ru</t>
+  </si>
+  <si>
+    <t>goney_axiyo89@aol.com</t>
+  </si>
+  <si>
+    <t>xuwu-tixiku76@mail.ru</t>
+  </si>
+  <si>
+    <t>wifin_icuhe96@yandex.ru</t>
+  </si>
+  <si>
+    <t>sozage_sefa55@yahoo.com</t>
+  </si>
+  <si>
+    <t>dogeta_sefu56@yandex.ru</t>
+  </si>
+  <si>
+    <t>zar-etosado40@yandex.ru</t>
+  </si>
+  <si>
+    <t>kahan_ecawi19@yandex.ru</t>
+  </si>
+  <si>
+    <t>danigit_ozi78@mail.ru</t>
+  </si>
+  <si>
+    <t>gusepa_libo96@mail.ru</t>
+  </si>
+  <si>
+    <t>zucuwit-ila20@yahoo.com</t>
+  </si>
+  <si>
+    <t>bupuvu-guja39@internet.ru</t>
+  </si>
+  <si>
+    <t>luyemi-vaji72@bk.ru</t>
+  </si>
+  <si>
+    <t>wix_asezisi8@internet.ru</t>
+  </si>
+  <si>
+    <t>kupapez-upa29@bk.ru</t>
+  </si>
+  <si>
+    <t>gilo_gexiki41@hotmail.com</t>
+  </si>
+  <si>
+    <t>jupo_wesaro47@yandex.ru</t>
+  </si>
+  <si>
+    <t>pabix-ariti1@yahoo.com</t>
+  </si>
+  <si>
+    <t>labu-bifazi81@yandex.ru</t>
+  </si>
+  <si>
+    <t>polalix-iwe35@internet.ru</t>
+  </si>
+  <si>
+    <t>tumum-eroze7@yahoo.com</t>
+  </si>
+  <si>
+    <t>sodiy-ujiyo99@internet.ru</t>
+  </si>
+  <si>
+    <t>sok-adeloju57@yandex.ru</t>
+  </si>
+  <si>
+    <t>tevazo-vupi40@aol.com</t>
+  </si>
+  <si>
+    <t>menino-dozo72@internet.ru</t>
+  </si>
+  <si>
+    <t>minut_emeza26@internet.ru</t>
+  </si>
+  <si>
+    <t>woyatu-zeki5@list.ru</t>
+  </si>
+  <si>
+    <t>neca-fodelo20@aol.com</t>
+  </si>
+  <si>
+    <t>zurin_usavi76@yahoo.com</t>
+  </si>
+  <si>
+    <t>yahomav-oyo7@gmail.com</t>
+  </si>
+  <si>
+    <t>kur-afazayi12@yandex.ru</t>
+  </si>
+  <si>
+    <t>loyugal-aja9@aol.com</t>
+  </si>
+  <si>
+    <t>haye-suwizu31@mail.ru</t>
+  </si>
+  <si>
+    <t>levosok-ode16@inbox.ru</t>
+  </si>
+  <si>
+    <t>vejisej-obo10@gmail.com</t>
+  </si>
+  <si>
+    <t>goy_epoloma41@list.ru</t>
+  </si>
+  <si>
+    <t>fetem-okozu92@bk.ru</t>
+  </si>
+  <si>
+    <t>fonuhos_ini86@mail.ru</t>
+  </si>
+  <si>
+    <t>sajudu-fika61@internet.ru</t>
+  </si>
+  <si>
+    <t>legi-nuvele58@internet.ru</t>
+  </si>
+  <si>
+    <t>gey_oveyuvi8@internet.ru</t>
+  </si>
+  <si>
+    <t>reravof-ece85@yahoo.com</t>
+  </si>
+  <si>
+    <t>yez-etitayi10@inbox.ru</t>
+  </si>
+  <si>
+    <t>mopa-vakimi67@gmail.com</t>
+  </si>
+  <si>
+    <t>huxej_olino44@inbox.ru</t>
+  </si>
+  <si>
+    <t>vefe-hudeja46@yahoo.com</t>
+  </si>
+  <si>
+    <t>yurokaj-ija46@yahoo.com</t>
+  </si>
+  <si>
+    <t>xug_evuvasi76@inbox.ru</t>
+  </si>
+  <si>
+    <t>jew_ehujabu99@yandex.ru</t>
+  </si>
+  <si>
+    <t>nud-iwubeje91@yahoo.com</t>
+  </si>
+  <si>
+    <t>lite_yapiya86@yahoo.com</t>
+  </si>
+  <si>
+    <t>kiced_ozija65@yahoo.com</t>
+  </si>
+  <si>
+    <t>nod-urowule27@mail.ru</t>
+  </si>
+  <si>
+    <t>juyij_ipogi99@aol.com</t>
+  </si>
+  <si>
+    <t>xiki-hanedo67@bk.ru</t>
+  </si>
+  <si>
+    <t>nayus_iwabi23@gmail.com</t>
+  </si>
+  <si>
+    <t>gan-ofekupo12@hotmail.com</t>
+  </si>
+  <si>
+    <t>sapij-ikelo22@mail.ru</t>
+  </si>
+  <si>
+    <t>zoyijil_ixo93@internet.ru</t>
+  </si>
+  <si>
+    <t>kar-ezazuku67@inbox.ru</t>
+  </si>
+  <si>
+    <t>peki-marupa81@hotmail.com</t>
+  </si>
+  <si>
+    <t>way_acalila86@aol.com</t>
+  </si>
+  <si>
+    <t>fihapex_eja73@hotmail.com</t>
+  </si>
+  <si>
+    <t>gijowu_vosa97@gmail.com</t>
+  </si>
+  <si>
+    <t>xese_horaha86@mail.ru</t>
+  </si>
+  <si>
+    <t>guh_ejopiwe1@yahoo.com</t>
+  </si>
+  <si>
+    <t>cosu_fajipa52@list.ru</t>
+  </si>
+  <si>
+    <t>lalafok-imu25@bk.ru</t>
+  </si>
+  <si>
+    <t>mefiju_kofa16@inbox.ru</t>
+  </si>
+  <si>
+    <t>nolifi_bama60@aol.com</t>
+  </si>
+  <si>
+    <t>wozat-awatu90@list.ru</t>
+  </si>
+  <si>
+    <t>tahibi_poha88@list.ru</t>
+  </si>
+  <si>
+    <t>geheha_goze46@gmail.com</t>
+  </si>
+  <si>
+    <t>lexokek-era33@mail.ru</t>
+  </si>
+  <si>
+    <t>zipupu_moye62@aol.com</t>
+  </si>
+  <si>
+    <t>bifuco_zite51@internet.ru</t>
+  </si>
+  <si>
+    <t>roye-kisora43@gmail.com</t>
+  </si>
+  <si>
+    <t>gelame-cogo20@list.ru</t>
+  </si>
+  <si>
+    <t>kuvu_nucovo46@hotmail.com</t>
+  </si>
+  <si>
+    <t>yoway-umeri94@inbox.ru</t>
+  </si>
+  <si>
+    <t>fepoc_ecele22@aol.com</t>
+  </si>
+  <si>
+    <t>rije-befugo71@gmail.com</t>
+  </si>
+  <si>
+    <t>baxe_gusure19@mail.ru</t>
+  </si>
+  <si>
+    <t>kusoki_yeki16@inbox.ru</t>
+  </si>
+  <si>
+    <t>nuzuza-sotu25@mail.ru</t>
+  </si>
+  <si>
+    <t>wulol_ejehe74@gmail.com</t>
+  </si>
+  <si>
+    <t>pat_ehukoga32@yandex.ru</t>
+  </si>
+  <si>
+    <t>wepu-fazuso77@aol.com</t>
+  </si>
+  <si>
+    <t>gorayey-ivi56@yahoo.com</t>
+  </si>
+  <si>
+    <t>saz_uwoberu21@bk.ru</t>
+  </si>
+  <si>
+    <t>kayavov-eyu62@list.ru</t>
+  </si>
+  <si>
+    <t>xofuh-atipu79@list.ru</t>
+  </si>
+  <si>
+    <t>ribukay-ipi34@yandex.ru</t>
+  </si>
+  <si>
+    <t>zaxavu_koti43@yahoo.com</t>
+  </si>
+  <si>
+    <t>yajej-asidi38@yahoo.com</t>
+  </si>
+  <si>
+    <t>sigapo-yumo83@internet.ru</t>
+  </si>
+  <si>
+    <t>xacov_ihaji56@list.ru</t>
+  </si>
+  <si>
+    <t>siwud-ebepe6@bk.ru</t>
+  </si>
+  <si>
+    <t>fabiraj_ewi60@mail.ru</t>
+  </si>
+  <si>
+    <t>zuduw_ihelu33@yahoo.com</t>
+  </si>
+  <si>
+    <t>tafagu_sora3@mail.ru</t>
+  </si>
+  <si>
+    <t>turuf-iwira64@aol.com</t>
+  </si>
+  <si>
+    <t>rajixu-giba34@bk.ru</t>
+  </si>
+  <si>
+    <t>wak_exanuro36@yahoo.com</t>
+  </si>
+  <si>
+    <t>yidubat-ede61@inbox.ru</t>
+  </si>
+  <si>
+    <t>vopu-dobeje30@yahoo.com</t>
+  </si>
+  <si>
+    <t>mikok_ifofu86@list.ru</t>
+  </si>
+  <si>
+    <t>sajidin_oge55@mail.ru</t>
+  </si>
+  <si>
+    <t>goti_kuhori62@gmail.com</t>
+  </si>
+  <si>
+    <t>lat_eyubunu44@list.ru</t>
+  </si>
+  <si>
+    <t>cose-zutujo86@gmail.com</t>
+  </si>
+  <si>
+    <t>jov_oxenide41@aol.com</t>
+  </si>
+  <si>
+    <t>taw-itodoxo12@mail.ru</t>
+  </si>
+  <si>
+    <t>foku-kibesu98@bk.ru</t>
+  </si>
+  <si>
+    <t>viy-okatowo2@aol.com</t>
+  </si>
+  <si>
+    <t>xubobo-joni21@bk.ru</t>
+  </si>
+  <si>
+    <t>zox_ufomuwa60@gmail.com</t>
+  </si>
+  <si>
+    <t>gos-iluledu23@internet.ru</t>
+  </si>
+  <si>
+    <t>koriv_uxifa25@internet.ru</t>
+  </si>
+  <si>
+    <t>saz-izeluku32@aol.com</t>
+  </si>
+  <si>
+    <t>kisodoy-oki94@inbox.ru</t>
+  </si>
+  <si>
+    <t>radikul_ehu92@yandex.ru</t>
+  </si>
+  <si>
+    <t>hama-pevayo33@internet.ru</t>
+  </si>
+  <si>
+    <t>cawifo_duha35@list.ru</t>
+  </si>
+  <si>
+    <t>zagobil_iho10@inbox.ru</t>
+  </si>
+  <si>
+    <t>somes-otuli5@internet.ru</t>
+  </si>
+  <si>
+    <t>dusaro-geto5@gmail.com</t>
+  </si>
+  <si>
+    <t>zelasu_xiwa26@gmail.com</t>
+  </si>
+  <si>
+    <t>gituf-evera95@yahoo.com</t>
+  </si>
+  <si>
+    <t>lule_vebigi42@mail.ru</t>
+  </si>
+  <si>
+    <t>jis-iredana58@gmail.com</t>
+  </si>
+  <si>
+    <t>lusema-vune41@bk.ru</t>
+  </si>
+  <si>
+    <t>dokede-gove37@gmail.com</t>
+  </si>
+  <si>
+    <t>nesatup-uwa16@bk.ru</t>
+  </si>
+  <si>
+    <t>powed_asobe66@gmail.com</t>
+  </si>
+  <si>
+    <t>nuxavu-seri52@mail.ru</t>
   </si>
 </sst>
 </file>
@@ -1666,20 +2308,21 @@
   </sheetPr>
   <dimension ref="A1:M1128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" customWidth="1"/>
     <col min="2" max="2" width="40.44140625" customWidth="1"/>
     <col min="3" max="3" width="45.109375" customWidth="1"/>
     <col min="4" max="4" width="30.109375" customWidth="1"/>
-    <col min="5" max="5" width="27.77734375" customWidth="1"/>
-    <col min="6" max="6" width="45.21875" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
+    <col min="6" max="6" width="45.33203125" customWidth="1"/>
     <col min="7" max="7" width="20.88671875" customWidth="1"/>
     <col min="12" max="12" width="33.44140625" customWidth="1"/>
+    <col min="13" max="13" width="22.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.2">
@@ -1752,6 +2395,9 @@
       <c r="L2" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="M2" t="s">
+        <v>438</v>
+      </c>
     </row>
     <row r="3" spans="1:13" ht="13.2">
       <c r="A3" s="1" t="s">
@@ -1784,6 +2430,9 @@
       <c r="L3" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="M3" t="s">
+        <v>439</v>
+      </c>
     </row>
     <row r="4" spans="1:13" ht="13.2">
       <c r="A4" s="1" t="s">
@@ -1818,6 +2467,9 @@
       <c r="L4" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="M4" t="s">
+        <v>440</v>
+      </c>
     </row>
     <row r="5" spans="1:13" ht="13.2">
       <c r="A5" s="1" t="s">
@@ -1852,6 +2504,9 @@
       <c r="L5" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="M5" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="6" spans="1:13" ht="13.2">
       <c r="A6" s="1" t="s">
@@ -1886,6 +2541,9 @@
       <c r="L6" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="M6" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="7" spans="1:13" ht="13.2">
       <c r="A7" s="1" t="s">
@@ -1920,6 +2578,9 @@
       <c r="L7" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="M7" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="8" spans="1:13" ht="13.2">
       <c r="A8" s="1" t="s">
@@ -1954,6 +2615,9 @@
       <c r="L8" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="M8" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="9" spans="1:13" ht="13.2">
       <c r="A9" s="1" t="s">
@@ -1988,6 +2652,9 @@
       <c r="L9" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="M9" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="10" spans="1:13" ht="13.2">
       <c r="A10" s="1" t="s">
@@ -2022,6 +2689,9 @@
       <c r="L10" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="M10" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="11" spans="1:13" ht="13.2">
       <c r="A11" s="1" t="s">
@@ -2056,6 +2726,9 @@
       <c r="L11" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="M11" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="12" spans="1:13" ht="13.2">
       <c r="A12" s="1" t="s">
@@ -2090,6 +2763,9 @@
       <c r="L12" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="M12" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="13" spans="1:13" ht="13.2">
       <c r="A13" s="1" t="s">
@@ -2124,6 +2800,9 @@
       <c r="L13" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="M13" t="s">
+        <v>449</v>
+      </c>
     </row>
     <row r="14" spans="1:13" ht="13.2">
       <c r="A14" s="1" t="s">
@@ -2158,6 +2837,9 @@
       <c r="L14" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="M14" t="s">
+        <v>450</v>
+      </c>
     </row>
     <row r="15" spans="1:13" ht="13.2">
       <c r="A15" s="1" t="s">
@@ -2192,6 +2874,9 @@
       <c r="L15" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="M15" t="s">
+        <v>451</v>
+      </c>
     </row>
     <row r="16" spans="1:13" ht="13.2">
       <c r="A16" s="1" t="s">
@@ -2226,8 +2911,11 @@
       <c r="L16" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="13.2">
+      <c r="M16" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="13.2">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -2260,8 +2948,11 @@
       <c r="L17" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="13.2">
+      <c r="M17" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="13.2">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -2294,8 +2985,11 @@
       <c r="L18" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="13.2">
+      <c r="M18" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="13.2">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -2328,8 +3022,11 @@
       <c r="L19" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="13.2">
+      <c r="M19" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="13.2">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
@@ -2362,8 +3059,11 @@
       <c r="L20" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="13.2">
+      <c r="M20" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="13.2">
       <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
@@ -2396,8 +3096,11 @@
       <c r="L21" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" ht="13.2">
+      <c r="M21" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="13.2">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
@@ -2430,8 +3133,11 @@
       <c r="L22" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" ht="13.2">
+      <c r="M22" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="13.2">
       <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
@@ -2464,8 +3170,11 @@
       <c r="L23" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" ht="13.2">
+      <c r="M23" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="13.2">
       <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
@@ -2498,8 +3207,11 @@
       <c r="L24" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" ht="13.2">
+      <c r="M24" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="13.2">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
@@ -2532,8 +3244,11 @@
       <c r="L25" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="13.2">
+      <c r="M25" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="13.2">
       <c r="A26" s="1" t="s">
         <v>13</v>
       </c>
@@ -2566,8 +3281,11 @@
       <c r="L26" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" ht="13.2">
+      <c r="M26" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="13.2">
       <c r="A27" s="1" t="s">
         <v>13</v>
       </c>
@@ -2600,8 +3318,11 @@
       <c r="L27" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" ht="13.2">
+      <c r="M27" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="13.2">
       <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
@@ -2634,8 +3355,11 @@
       <c r="L28" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" ht="13.2">
+      <c r="M28" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="13.2">
       <c r="A29" s="1" t="s">
         <v>13</v>
       </c>
@@ -2668,8 +3392,11 @@
       <c r="L29" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" ht="13.2">
+      <c r="M29" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="13.2">
       <c r="A30" s="1" t="s">
         <v>13</v>
       </c>
@@ -2702,8 +3429,11 @@
       <c r="L30" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" ht="13.2">
+      <c r="M30" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="13.2">
       <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
@@ -2736,8 +3466,11 @@
       <c r="L31" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" ht="13.2">
+      <c r="M31" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="13.2">
       <c r="A32" s="1" t="s">
         <v>13</v>
       </c>
@@ -2770,8 +3503,11 @@
       <c r="L32" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" ht="13.2">
+      <c r="M32" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="13.2">
       <c r="A33" s="1" t="s">
         <v>13</v>
       </c>
@@ -2802,8 +3538,11 @@
       <c r="L33" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" ht="13.2">
+      <c r="M33" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="13.2">
       <c r="A34" s="1" t="s">
         <v>13</v>
       </c>
@@ -2836,8 +3575,11 @@
       <c r="L34" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" ht="13.2">
+      <c r="M34" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="13.2">
       <c r="A35" s="1" t="s">
         <v>13</v>
       </c>
@@ -2872,8 +3614,11 @@
       <c r="L35" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" ht="13.2">
+      <c r="M35" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="13.2">
       <c r="A36" s="1" t="s">
         <v>13</v>
       </c>
@@ -2908,8 +3653,11 @@
       <c r="L36" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" ht="13.2">
+      <c r="M36" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="13.2">
       <c r="A37" s="1" t="s">
         <v>13</v>
       </c>
@@ -2944,8 +3692,11 @@
       <c r="L37" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" ht="13.2">
+      <c r="M37" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="13.2">
       <c r="A38" s="1" t="s">
         <v>13</v>
       </c>
@@ -2980,8 +3731,11 @@
       <c r="L38" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" ht="13.2">
+      <c r="M38" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="13.2">
       <c r="A39" s="1" t="s">
         <v>13</v>
       </c>
@@ -3016,8 +3770,11 @@
       <c r="L39" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" ht="13.2">
+      <c r="M39" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="13.2">
       <c r="A40" s="1" t="s">
         <v>13</v>
       </c>
@@ -3052,8 +3809,11 @@
       <c r="L40" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" ht="13.2">
+      <c r="M40" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="13.2">
       <c r="A41" s="1" t="s">
         <v>13</v>
       </c>
@@ -3088,8 +3848,11 @@
       <c r="L41" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" ht="13.2">
+      <c r="M41" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="13.2">
       <c r="A42" s="1" t="s">
         <v>13</v>
       </c>
@@ -3124,8 +3887,11 @@
       <c r="L42" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" ht="13.2">
+      <c r="M42" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="13.2">
       <c r="A43" s="1" t="s">
         <v>13</v>
       </c>
@@ -3160,8 +3926,11 @@
       <c r="L43" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" ht="13.2">
+      <c r="M43" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="13.2">
       <c r="A44" s="1" t="s">
         <v>13</v>
       </c>
@@ -3196,8 +3965,11 @@
       <c r="L44" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" ht="13.2">
+      <c r="M44" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="13.2">
       <c r="A45" s="1" t="s">
         <v>13</v>
       </c>
@@ -3232,8 +4004,11 @@
       <c r="L45" s="1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" ht="13.2">
+      <c r="M45" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="13.2">
       <c r="A46" s="1" t="s">
         <v>13</v>
       </c>
@@ -3268,8 +4043,11 @@
       <c r="L46" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" ht="13.2">
+      <c r="M46" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="13.2">
       <c r="A47" s="1" t="s">
         <v>13</v>
       </c>
@@ -3304,8 +4082,11 @@
       <c r="L47" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" ht="13.2">
+      <c r="M47" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="13.2">
       <c r="A48" s="1" t="s">
         <v>13</v>
       </c>
@@ -3340,8 +4121,11 @@
       <c r="L48" s="1" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" ht="13.2">
+      <c r="M48" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="13.2">
       <c r="A49" s="1" t="s">
         <v>13</v>
       </c>
@@ -3376,8 +4160,11 @@
       <c r="L49" s="1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" ht="13.2">
+      <c r="M49" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="13.2">
       <c r="A50" s="1" t="s">
         <v>13</v>
       </c>
@@ -3412,8 +4199,11 @@
       <c r="L50" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" ht="13.2">
+      <c r="M50" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="13.2">
       <c r="A51" s="1" t="s">
         <v>13</v>
       </c>
@@ -3448,8 +4238,11 @@
       <c r="L51" s="1" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" ht="13.2">
+      <c r="M51" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="13.2">
       <c r="A52" s="1" t="s">
         <v>13</v>
       </c>
@@ -3484,8 +4277,11 @@
       <c r="L52" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" ht="13.2">
+      <c r="M52" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="13.2">
       <c r="A53" s="1" t="s">
         <v>13</v>
       </c>
@@ -3520,8 +4316,11 @@
       <c r="L53" s="1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" ht="13.2">
+      <c r="M53" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="13.2">
       <c r="A54" s="1" t="s">
         <v>13</v>
       </c>
@@ -3556,8 +4355,11 @@
       <c r="L54" s="1" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" ht="13.2">
+      <c r="M54" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="13.2">
       <c r="A55" s="1" t="s">
         <v>13</v>
       </c>
@@ -3592,8 +4394,11 @@
       <c r="L55" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" ht="13.2">
+      <c r="M55" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="13.2">
       <c r="A56" s="1" t="s">
         <v>13</v>
       </c>
@@ -3628,8 +4433,11 @@
       <c r="L56" s="1" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" ht="13.2">
+      <c r="M56" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="13.2">
       <c r="A57" s="1" t="s">
         <v>13</v>
       </c>
@@ -3664,8 +4472,11 @@
       <c r="L57" s="1" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" ht="13.2">
+      <c r="M57" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="13.2">
       <c r="A58" s="1" t="s">
         <v>13</v>
       </c>
@@ -3700,8 +4511,11 @@
       <c r="L58" s="1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" ht="13.2">
+      <c r="M58" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="13.2">
       <c r="A59" s="1" t="s">
         <v>13</v>
       </c>
@@ -3736,8 +4550,11 @@
       <c r="L59" s="1" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" ht="13.2">
+      <c r="M59" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="13.2">
       <c r="A60" s="1" t="s">
         <v>13</v>
       </c>
@@ -3772,8 +4589,11 @@
       <c r="L60" s="1" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" ht="13.2">
+      <c r="M60" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="13.2">
       <c r="A61" s="1" t="s">
         <v>13</v>
       </c>
@@ -3806,8 +4626,11 @@
       <c r="L61" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" ht="13.2">
+      <c r="M61" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="13.2">
       <c r="A62" s="1" t="s">
         <v>13</v>
       </c>
@@ -3840,8 +4663,11 @@
       <c r="L62" s="1" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" ht="13.2">
+      <c r="M62" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="13.2">
       <c r="A63" s="1" t="s">
         <v>13</v>
       </c>
@@ -3874,8 +4700,11 @@
       <c r="L63" s="1" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" ht="13.2">
+      <c r="M63" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="13.2">
       <c r="A64" s="1" t="s">
         <v>13</v>
       </c>
@@ -3908,8 +4737,11 @@
       <c r="L64" s="1" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" ht="13.2">
+      <c r="M64" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="13.2">
       <c r="A65" s="1" t="s">
         <v>13</v>
       </c>
@@ -3942,8 +4774,11 @@
       <c r="L65" s="1" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" ht="13.2">
+      <c r="M65" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="13.2">
       <c r="A66" s="1" t="s">
         <v>13</v>
       </c>
@@ -3976,8 +4811,11 @@
       <c r="L66" s="1" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" ht="13.2">
+      <c r="M66" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="13.2">
       <c r="A67" s="1" t="s">
         <v>13</v>
       </c>
@@ -4010,8 +4848,11 @@
       <c r="L67" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" ht="13.2">
+      <c r="M67" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="13.2">
       <c r="A68" s="1" t="s">
         <v>222</v>
       </c>
@@ -4040,8 +4881,11 @@
       <c r="L68" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" ht="16.5" customHeight="1">
+      <c r="M68" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="16.5" customHeight="1">
       <c r="A69" s="1" t="s">
         <v>222</v>
       </c>
@@ -4072,8 +4916,11 @@
       <c r="L69" s="1" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" ht="13.2">
+      <c r="M69" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="13.2">
       <c r="A70" s="1" t="s">
         <v>222</v>
       </c>
@@ -4106,8 +4953,11 @@
       <c r="L70" s="1" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" ht="13.2">
+      <c r="M70" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="13.2">
       <c r="A71" s="1" t="s">
         <v>222</v>
       </c>
@@ -4142,8 +4992,11 @@
       <c r="L71" s="1" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="72" spans="1:12" ht="13.2">
+      <c r="M71" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="13.2">
       <c r="A72" s="1" t="s">
         <v>222</v>
       </c>
@@ -4178,8 +5031,11 @@
       <c r="L72" s="1" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" ht="13.2">
+      <c r="M72" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" ht="13.2">
       <c r="A73" s="1" t="s">
         <v>222</v>
       </c>
@@ -4214,8 +5070,11 @@
       <c r="L73" s="1" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" ht="13.2">
+      <c r="M73" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" ht="13.2">
       <c r="A74" s="1" t="s">
         <v>222</v>
       </c>
@@ -4250,8 +5109,11 @@
       <c r="L74" s="1" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="75" spans="1:12" ht="13.2">
+      <c r="M74" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="13.2">
       <c r="A75" s="1" t="s">
         <v>222</v>
       </c>
@@ -4286,8 +5148,11 @@
       <c r="L75" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" ht="13.2">
+      <c r="M75" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="13.2">
       <c r="A76" s="1" t="s">
         <v>222</v>
       </c>
@@ -4322,8 +5187,11 @@
       <c r="L76" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="77" spans="1:12" ht="13.2">
+      <c r="M76" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" ht="13.2">
       <c r="A77" s="1" t="s">
         <v>222</v>
       </c>
@@ -4358,8 +5226,11 @@
       <c r="L77" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="78" spans="1:12" ht="13.2">
+      <c r="M77" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" ht="13.2">
       <c r="A78" s="1" t="s">
         <v>222</v>
       </c>
@@ -4394,8 +5265,11 @@
       <c r="L78" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" ht="13.2">
+      <c r="M78" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="13.2">
       <c r="A79" s="1" t="s">
         <v>222</v>
       </c>
@@ -4430,8 +5304,11 @@
       <c r="L79" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" ht="13.2">
+      <c r="M79" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" ht="13.2">
       <c r="A80" s="1" t="s">
         <v>222</v>
       </c>
@@ -4466,8 +5343,11 @@
       <c r="L80" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="81" spans="1:12" ht="13.2">
+      <c r="M80" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" ht="13.2">
       <c r="A81" s="1" t="s">
         <v>222</v>
       </c>
@@ -4502,8 +5382,11 @@
       <c r="L81" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" ht="13.2">
+      <c r="M81" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" ht="13.2">
       <c r="A82" s="1" t="s">
         <v>222</v>
       </c>
@@ -4538,8 +5421,11 @@
       <c r="L82" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" ht="13.2">
+      <c r="M82" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" ht="13.2">
       <c r="A83" s="1" t="s">
         <v>222</v>
       </c>
@@ -4574,8 +5460,11 @@
       <c r="L83" s="1" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="84" spans="1:12" ht="16.5" customHeight="1">
+      <c r="M83" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" ht="16.5" customHeight="1">
       <c r="A84" s="1" t="s">
         <v>222</v>
       </c>
@@ -4610,8 +5499,11 @@
       <c r="L84" s="1" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" ht="16.5" customHeight="1">
+      <c r="M84" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" ht="16.5" customHeight="1">
       <c r="A85" s="1" t="s">
         <v>222</v>
       </c>
@@ -4646,8 +5538,11 @@
       <c r="L85" s="1" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="86" spans="1:12" ht="16.5" customHeight="1">
+      <c r="M85" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" ht="16.5" customHeight="1">
       <c r="A86" s="1" t="s">
         <v>222</v>
       </c>
@@ -4682,8 +5577,11 @@
       <c r="L86" s="1" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="87" spans="1:12" ht="16.5" customHeight="1">
+      <c r="M86" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" ht="16.5" customHeight="1">
       <c r="A87" s="1" t="s">
         <v>222</v>
       </c>
@@ -4718,8 +5616,11 @@
       <c r="L87" s="1" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="88" spans="1:12" ht="16.5" customHeight="1">
+      <c r="M87" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" ht="16.5" customHeight="1">
       <c r="A88" s="1" t="s">
         <v>222</v>
       </c>
@@ -4752,8 +5653,11 @@
       <c r="L88" s="1" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="89" spans="1:12" ht="16.5" customHeight="1">
+      <c r="M88" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" ht="16.5" customHeight="1">
       <c r="A89" s="1" t="s">
         <v>222</v>
       </c>
@@ -4788,8 +5692,11 @@
       <c r="L89" s="1" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="90" spans="1:12" ht="16.5" customHeight="1">
+      <c r="M89" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" ht="16.5" customHeight="1">
       <c r="A90" s="1" t="s">
         <v>222</v>
       </c>
@@ -4824,8 +5731,11 @@
       <c r="L90" s="1" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="91" spans="1:12" ht="16.5" customHeight="1">
+      <c r="M90" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" ht="16.5" customHeight="1">
       <c r="A91" s="1" t="s">
         <v>222</v>
       </c>
@@ -4860,8 +5770,11 @@
       <c r="L91" s="1" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="92" spans="1:12" ht="13.2">
+      <c r="M91" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" ht="13.2">
       <c r="A92" s="1" t="s">
         <v>222</v>
       </c>
@@ -4896,8 +5809,11 @@
       <c r="L92" s="1" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="93" spans="1:12" ht="13.2">
+      <c r="M92" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" ht="13.2">
       <c r="A93" s="1" t="s">
         <v>222</v>
       </c>
@@ -4932,8 +5848,11 @@
       <c r="L93" s="1" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="94" spans="1:12" ht="13.2">
+      <c r="M93" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" ht="13.2">
       <c r="A94" s="1" t="s">
         <v>222</v>
       </c>
@@ -4968,8 +5887,11 @@
       <c r="L94" s="1" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="95" spans="1:12" ht="13.2">
+      <c r="M94" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" ht="13.2">
       <c r="A95" s="1" t="s">
         <v>222</v>
       </c>
@@ -5004,8 +5926,11 @@
       <c r="L95" s="1" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="96" spans="1:12" ht="13.2">
+      <c r="M95" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" ht="13.2">
       <c r="A96" s="1" t="s">
         <v>222</v>
       </c>
@@ -5040,8 +5965,11 @@
       <c r="L96" s="1" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="97" spans="1:12" ht="13.2">
+      <c r="M96" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" ht="13.2">
       <c r="A97" s="1" t="s">
         <v>222</v>
       </c>
@@ -5076,8 +6004,11 @@
       <c r="L97" s="1" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="98" spans="1:12" ht="13.2">
+      <c r="M97" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" ht="13.2">
       <c r="A98" s="1" t="s">
         <v>222</v>
       </c>
@@ -5112,8 +6043,11 @@
       <c r="L98" s="1" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="99" spans="1:12" ht="13.2">
+      <c r="M98" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" ht="13.2">
       <c r="A99" s="1" t="s">
         <v>222</v>
       </c>
@@ -5148,8 +6082,11 @@
       <c r="L99" s="1" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="100" spans="1:12" ht="13.2">
+      <c r="M99" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" ht="13.2">
       <c r="A100" s="1" t="s">
         <v>222</v>
       </c>
@@ -5184,8 +6121,11 @@
       <c r="L100" s="1" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="101" spans="1:12" ht="13.2">
+      <c r="M100" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" ht="13.2">
       <c r="A101" s="1" t="s">
         <v>222</v>
       </c>
@@ -5220,8 +6160,11 @@
       <c r="L101" s="1" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="102" spans="1:12" ht="13.2">
+      <c r="M101" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" ht="13.2">
       <c r="A102" s="1" t="s">
         <v>222</v>
       </c>
@@ -5256,8 +6199,11 @@
       <c r="L102" s="1" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="103" spans="1:12" ht="13.2">
+      <c r="M102" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" ht="13.2">
       <c r="A103" s="1" t="s">
         <v>222</v>
       </c>
@@ -5292,8 +6238,11 @@
       <c r="L103" s="1" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="104" spans="1:12" ht="13.2">
+      <c r="M103" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" ht="13.2">
       <c r="A104" s="1" t="s">
         <v>222</v>
       </c>
@@ -5328,8 +6277,11 @@
       <c r="L104" s="1" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="105" spans="1:12" ht="13.2">
+      <c r="M104" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" ht="13.2">
       <c r="A105" s="1" t="s">
         <v>222</v>
       </c>
@@ -5360,8 +6312,11 @@
       <c r="L105" s="1" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="106" spans="1:12" ht="13.2">
+      <c r="M105" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" ht="13.2">
       <c r="A106" s="1" t="s">
         <v>222</v>
       </c>
@@ -5394,8 +6349,11 @@
       <c r="L106" s="1" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="107" spans="1:12" ht="13.2">
+      <c r="M106" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" ht="13.2">
       <c r="A107" s="1" t="s">
         <v>222</v>
       </c>
@@ -5428,8 +6386,11 @@
       <c r="L107" s="1" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="108" spans="1:12" ht="13.2">
+      <c r="M107" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" ht="13.2">
       <c r="A108" s="1" t="s">
         <v>222</v>
       </c>
@@ -5462,8 +6423,11 @@
       <c r="L108" s="1" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="109" spans="1:12" ht="13.2">
+      <c r="M108" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" ht="13.2">
       <c r="A109" s="1" t="s">
         <v>222</v>
       </c>
@@ -5496,8 +6460,11 @@
       <c r="L109" s="1" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="110" spans="1:12" ht="13.2">
+      <c r="M109" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" ht="13.2">
       <c r="A110" s="1" t="s">
         <v>222</v>
       </c>
@@ -5530,8 +6497,11 @@
       <c r="L110" s="1" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="111" spans="1:12" ht="13.2">
+      <c r="M110" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" ht="13.2">
       <c r="A111" s="1" t="s">
         <v>222</v>
       </c>
@@ -5564,8 +6534,11 @@
       <c r="L111" s="1" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="112" spans="1:12" ht="13.2">
+      <c r="M111" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" ht="13.2">
       <c r="A112" s="1" t="s">
         <v>222</v>
       </c>
@@ -5598,8 +6571,11 @@
       <c r="L112" s="1" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="113" spans="1:12" ht="13.2">
+      <c r="M112" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" ht="13.2">
       <c r="A113" s="1" t="s">
         <v>222</v>
       </c>
@@ -5632,8 +6608,11 @@
       <c r="L113" s="1" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="114" spans="1:12" ht="13.2">
+      <c r="M113" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" ht="13.2">
       <c r="A114" s="1" t="s">
         <v>222</v>
       </c>
@@ -5666,8 +6645,11 @@
       <c r="L114" s="1" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="115" spans="1:12" ht="13.2">
+      <c r="M114" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" ht="13.2">
       <c r="A115" s="1" t="s">
         <v>222</v>
       </c>
@@ -5700,8 +6682,11 @@
       <c r="L115" s="1" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="116" spans="1:12" ht="13.2">
+      <c r="M115" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" ht="13.2">
       <c r="A116" s="1" t="s">
         <v>222</v>
       </c>
@@ -5734,8 +6719,11 @@
       <c r="L116" s="1" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="117" spans="1:12" ht="13.2">
+      <c r="M116" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" ht="13.2">
       <c r="A117" s="1" t="s">
         <v>222</v>
       </c>
@@ -5768,8 +6756,11 @@
       <c r="L117" s="1" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="118" spans="1:12" ht="13.2">
+      <c r="M117" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" ht="13.2">
       <c r="A118" s="1" t="s">
         <v>222</v>
       </c>
@@ -5802,8 +6793,11 @@
       <c r="L118" s="1" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="119" spans="1:12" ht="13.2">
+      <c r="M118" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" ht="13.2">
       <c r="A119" s="1" t="s">
         <v>222</v>
       </c>
@@ -5835,8 +6829,11 @@
       <c r="L119" s="1" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="120" spans="1:12" ht="13.2">
+      <c r="M119" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" ht="13.2">
       <c r="A120" s="1" t="s">
         <v>222</v>
       </c>
@@ -5868,8 +6865,11 @@
       <c r="L120" s="1" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="121" spans="1:12" ht="13.2">
+      <c r="M120" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" ht="13.2">
       <c r="A121" s="1" t="s">
         <v>222</v>
       </c>
@@ -5901,8 +6901,11 @@
       <c r="L121" s="1" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="122" spans="1:12" ht="13.2">
+      <c r="M121" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" ht="13.2">
       <c r="A122" s="1" t="s">
         <v>222</v>
       </c>
@@ -5934,8 +6937,11 @@
       <c r="L122" s="1" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="123" spans="1:12" ht="13.2">
+      <c r="M122" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" ht="13.2">
       <c r="A123" s="1" t="s">
         <v>222</v>
       </c>
@@ -5967,8 +6973,11 @@
       <c r="L123" s="1" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="124" spans="1:12" ht="13.2">
+      <c r="M123" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" ht="13.2">
       <c r="A124" s="1" t="s">
         <v>222</v>
       </c>
@@ -6000,8 +7009,11 @@
       <c r="L124" s="1" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="125" spans="1:12" ht="13.2">
+      <c r="M124" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" ht="13.2">
       <c r="A125" s="1" t="s">
         <v>222</v>
       </c>
@@ -6033,8 +7045,11 @@
       <c r="L125" s="1" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="126" spans="1:12" ht="13.2">
+      <c r="M125" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" ht="13.2">
       <c r="A126" s="1" t="s">
         <v>222</v>
       </c>
@@ -6066,8 +7081,11 @@
       <c r="L126" s="1" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="127" spans="1:12" ht="13.2">
+      <c r="M126" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" ht="13.2">
       <c r="A127" s="1" t="s">
         <v>222</v>
       </c>
@@ -6099,8 +7117,11 @@
       <c r="L127" s="1" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="128" spans="1:12" ht="13.2">
+      <c r="M127" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" ht="13.2">
       <c r="A128" s="1" t="s">
         <v>222</v>
       </c>
@@ -6132,8 +7153,11 @@
       <c r="L128" s="1" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="129" spans="1:12" ht="13.2">
+      <c r="M128" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" ht="13.2">
       <c r="A129" s="1" t="s">
         <v>222</v>
       </c>
@@ -6165,8 +7189,11 @@
       <c r="L129" s="1" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="130" spans="1:12" ht="13.2">
+      <c r="M129" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" ht="13.2">
       <c r="A130" s="1" t="s">
         <v>222</v>
       </c>
@@ -6198,8 +7225,11 @@
       <c r="L130" s="1" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="131" spans="1:12" ht="13.2">
+      <c r="M130" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" ht="13.2">
       <c r="A131" s="1" t="s">
         <v>222</v>
       </c>
@@ -6231,8 +7261,11 @@
       <c r="L131" s="1" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="132" spans="1:12" ht="13.2">
+      <c r="M131" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" ht="13.2">
       <c r="A132" s="1" t="s">
         <v>222</v>
       </c>
@@ -6264,8 +7297,11 @@
       <c r="L132" s="1" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="133" spans="1:12" ht="13.2">
+      <c r="M132" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" ht="13.2">
       <c r="A133" s="1" t="s">
         <v>222</v>
       </c>
@@ -6297,8 +7333,11 @@
       <c r="L133" s="1" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="134" spans="1:12" ht="13.2">
+      <c r="M133" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" ht="13.2">
       <c r="A134" s="1" t="s">
         <v>222</v>
       </c>
@@ -6330,8 +7369,11 @@
       <c r="L134" s="1" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="135" spans="1:12" ht="13.2">
+      <c r="M134" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" ht="13.2">
       <c r="A135" s="1" t="s">
         <v>222</v>
       </c>
@@ -6363,8 +7405,11 @@
       <c r="L135" s="1" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="136" spans="1:12" ht="13.2">
+      <c r="M135" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" ht="13.2">
       <c r="A136" s="1" t="s">
         <v>222</v>
       </c>
@@ -6396,8 +7441,11 @@
       <c r="L136" s="1" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="137" spans="1:12" ht="13.2">
+      <c r="M136" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" ht="13.2">
       <c r="A137" s="1" t="s">
         <v>222</v>
       </c>
@@ -6429,8 +7477,11 @@
       <c r="L137" s="1" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="138" spans="1:12" ht="13.2">
+      <c r="M137" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" ht="13.2">
       <c r="A138" s="1" t="s">
         <v>222</v>
       </c>
@@ -6462,8 +7513,11 @@
       <c r="L138" s="1" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="139" spans="1:12" ht="13.2">
+      <c r="M138" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" ht="13.2">
       <c r="A139" s="1" t="s">
         <v>222</v>
       </c>
@@ -6495,8 +7549,11 @@
       <c r="L139" s="1" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="140" spans="1:12" ht="13.2">
+      <c r="M139" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" ht="13.2">
       <c r="A140" s="1" t="s">
         <v>222</v>
       </c>
@@ -6528,8 +7585,11 @@
       <c r="L140" s="1" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="141" spans="1:12" ht="13.2">
+      <c r="M140" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" ht="13.2">
       <c r="A141" s="1" t="s">
         <v>222</v>
       </c>
@@ -6561,8 +7621,11 @@
       <c r="L141" s="1" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="142" spans="1:12" ht="13.2">
+      <c r="M141" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" ht="13.2">
       <c r="A142" s="1" t="s">
         <v>222</v>
       </c>
@@ -6594,8 +7657,11 @@
       <c r="L142" s="1" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="143" spans="1:12" ht="13.2">
+      <c r="M142" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" ht="13.2">
       <c r="A143" s="1" t="s">
         <v>222</v>
       </c>
@@ -6627,8 +7693,11 @@
       <c r="L143" s="1" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="144" spans="1:12" ht="13.2">
+      <c r="M143" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" ht="13.2">
       <c r="A144" s="1" t="s">
         <v>222</v>
       </c>
@@ -6660,8 +7729,11 @@
       <c r="L144" s="1" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="145" spans="1:12" ht="13.2">
+      <c r="M144" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" ht="13.2">
       <c r="A145" s="1" t="s">
         <v>354</v>
       </c>
@@ -6690,8 +7762,11 @@
       <c r="L145" s="1" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="146" spans="1:12" ht="13.2">
+      <c r="M145" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" ht="13.2">
       <c r="A146" s="1" t="s">
         <v>354</v>
       </c>
@@ -6722,8 +7797,11 @@
       <c r="L146" s="1" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="147" spans="1:12" ht="13.2">
+      <c r="M146" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" ht="13.2">
       <c r="A147" s="1" t="s">
         <v>354</v>
       </c>
@@ -6756,8 +7834,11 @@
       <c r="L147" s="1" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="148" spans="1:12" ht="13.2">
+      <c r="M147" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" ht="13.2">
       <c r="A148" s="1" t="s">
         <v>354</v>
       </c>
@@ -6792,8 +7873,11 @@
       <c r="L148" s="1" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="149" spans="1:12" ht="13.2">
+      <c r="M148" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" ht="13.2">
       <c r="A149" s="1" t="s">
         <v>354</v>
       </c>
@@ -6828,8 +7912,11 @@
       <c r="L149" s="1" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="150" spans="1:12" ht="13.2">
+      <c r="M149" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" ht="13.2">
       <c r="A150" s="1" t="s">
         <v>354</v>
       </c>
@@ -6864,8 +7951,11 @@
       <c r="L150" s="1" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="151" spans="1:12" ht="13.2">
+      <c r="M150" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" ht="13.2">
       <c r="A151" s="1" t="s">
         <v>354</v>
       </c>
@@ -6900,8 +7990,11 @@
       <c r="L151" s="1" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="152" spans="1:12" ht="13.2">
+      <c r="M151" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" ht="13.2">
       <c r="A152" s="1" t="s">
         <v>354</v>
       </c>
@@ -6936,8 +8029,11 @@
       <c r="L152" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="153" spans="1:12" ht="13.2">
+      <c r="M152" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" ht="13.2">
       <c r="A153" s="1" t="s">
         <v>354</v>
       </c>
@@ -6972,8 +8068,11 @@
       <c r="L153" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="154" spans="1:12" ht="13.2">
+      <c r="M153" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" ht="13.2">
       <c r="A154" s="1" t="s">
         <v>354</v>
       </c>
@@ -7008,8 +8107,11 @@
       <c r="L154" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="155" spans="1:12" ht="13.2">
+      <c r="M154" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" ht="13.2">
       <c r="A155" s="1" t="s">
         <v>354</v>
       </c>
@@ -7044,8 +8146,11 @@
       <c r="L155" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="156" spans="1:12" ht="13.2">
+      <c r="M155" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" ht="13.2">
       <c r="A156" s="1" t="s">
         <v>354</v>
       </c>
@@ -7080,8 +8185,11 @@
       <c r="L156" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="157" spans="1:12" ht="13.2">
+      <c r="M156" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" ht="13.2">
       <c r="A157" s="1" t="s">
         <v>354</v>
       </c>
@@ -7116,8 +8224,11 @@
       <c r="L157" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="158" spans="1:12" ht="13.2">
+      <c r="M157" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" ht="13.2">
       <c r="A158" s="1" t="s">
         <v>354</v>
       </c>
@@ -7152,8 +8263,11 @@
       <c r="L158" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="159" spans="1:12" ht="13.2">
+      <c r="M158" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" ht="13.2">
       <c r="A159" s="1" t="s">
         <v>354</v>
       </c>
@@ -7188,8 +8302,11 @@
       <c r="L159" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="160" spans="1:12" ht="13.2">
+      <c r="M159" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" ht="13.2">
       <c r="A160" s="1" t="s">
         <v>354</v>
       </c>
@@ -7224,8 +8341,11 @@
       <c r="L160" s="1" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="161" spans="1:12" ht="13.2">
+      <c r="M160" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" ht="13.2">
       <c r="A161" s="1" t="s">
         <v>354</v>
       </c>
@@ -7260,8 +8380,11 @@
       <c r="L161" s="1" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="162" spans="1:12" ht="13.2">
+      <c r="M161" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" ht="13.2">
       <c r="A162" s="1" t="s">
         <v>354</v>
       </c>
@@ -7296,8 +8419,11 @@
       <c r="L162" s="1" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="163" spans="1:12" ht="13.2">
+      <c r="M162" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" ht="13.2">
       <c r="A163" s="1" t="s">
         <v>354</v>
       </c>
@@ -7332,8 +8458,11 @@
       <c r="L163" s="1" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="164" spans="1:12" ht="13.2">
+      <c r="M163" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" ht="13.2">
       <c r="A164" s="1" t="s">
         <v>354</v>
       </c>
@@ -7368,8 +8497,11 @@
       <c r="L164" s="1" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="165" spans="1:12" ht="13.2">
+      <c r="M164" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" ht="13.2">
       <c r="A165" s="1" t="s">
         <v>354</v>
       </c>
@@ -7402,8 +8534,11 @@
       <c r="L165" s="1" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="166" spans="1:12" ht="13.2">
+      <c r="M165" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" ht="13.2">
       <c r="A166" s="1" t="s">
         <v>354</v>
       </c>
@@ -7438,8 +8573,11 @@
       <c r="L166" s="1" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="167" spans="1:12" ht="13.2">
+      <c r="M166" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" ht="13.2">
       <c r="A167" s="1" t="s">
         <v>354</v>
       </c>
@@ -7474,8 +8612,11 @@
       <c r="L167" s="1" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="168" spans="1:12" ht="13.2">
+      <c r="M167" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" ht="13.2">
       <c r="A168" s="1" t="s">
         <v>354</v>
       </c>
@@ -7510,8 +8651,11 @@
       <c r="L168" s="1" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="169" spans="1:12" ht="13.2">
+      <c r="M168" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" ht="13.2">
       <c r="A169" s="1" t="s">
         <v>354</v>
       </c>
@@ -7546,8 +8690,11 @@
       <c r="L169" s="1" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="170" spans="1:12" ht="13.2">
+      <c r="M169" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" ht="13.2">
       <c r="A170" s="1" t="s">
         <v>354</v>
       </c>
@@ -7582,8 +8729,11 @@
       <c r="L170" s="1" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="171" spans="1:12" ht="13.2">
+      <c r="M170" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" ht="13.2">
       <c r="A171" s="1" t="s">
         <v>354</v>
       </c>
@@ -7618,8 +8768,11 @@
       <c r="L171" s="1" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="172" spans="1:12" ht="13.2">
+      <c r="M171" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" ht="13.2">
       <c r="A172" s="1" t="s">
         <v>354</v>
       </c>
@@ -7654,8 +8807,11 @@
       <c r="L172" s="1" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="173" spans="1:12" ht="13.2">
+      <c r="M172" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" ht="13.2">
       <c r="A173" s="1" t="s">
         <v>354</v>
       </c>
@@ -7690,8 +8846,11 @@
       <c r="L173" s="1" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="174" spans="1:12" ht="13.2">
+      <c r="M173" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" ht="13.2">
       <c r="A174" s="1" t="s">
         <v>354</v>
       </c>
@@ -7726,8 +8885,11 @@
       <c r="L174" s="1" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="175" spans="1:12" ht="13.2">
+      <c r="M174" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" ht="13.2">
       <c r="A175" s="1" t="s">
         <v>354</v>
       </c>
@@ -7762,8 +8924,11 @@
       <c r="L175" s="1" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="176" spans="1:12" ht="13.2">
+      <c r="M175" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" ht="13.2">
       <c r="A176" s="1" t="s">
         <v>354</v>
       </c>
@@ -7798,8 +8963,11 @@
       <c r="L176" s="1" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="177" spans="1:12" ht="13.2">
+      <c r="M176" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" ht="13.2">
       <c r="A177" s="1" t="s">
         <v>354</v>
       </c>
@@ -7834,8 +9002,11 @@
       <c r="L177" s="1" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="178" spans="1:12" ht="13.2">
+      <c r="M177" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" ht="13.2">
       <c r="A178" s="1" t="s">
         <v>354</v>
       </c>
@@ -7870,8 +9041,11 @@
       <c r="L178" s="1" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="179" spans="1:12" ht="13.2">
+      <c r="M178" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" ht="13.2">
       <c r="A179" s="1" t="s">
         <v>354</v>
       </c>
@@ -7902,8 +9076,11 @@
       <c r="L179" s="1" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="180" spans="1:12" ht="13.2">
+      <c r="M179" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" ht="13.2">
       <c r="A180" s="1" t="s">
         <v>354</v>
       </c>
@@ -7936,8 +9113,11 @@
       <c r="L180" s="1" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="181" spans="1:12" ht="13.2">
+      <c r="M180" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" ht="13.2">
       <c r="A181" s="1" t="s">
         <v>354</v>
       </c>
@@ -7970,8 +9150,11 @@
       <c r="L181" s="1" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="182" spans="1:12" ht="13.2">
+      <c r="M181" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" ht="13.2">
       <c r="A182" s="1" t="s">
         <v>354</v>
       </c>
@@ -8004,8 +9187,11 @@
       <c r="L182" s="1" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="183" spans="1:12" ht="13.2">
+      <c r="M182" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" ht="13.2">
       <c r="A183" s="1" t="s">
         <v>354</v>
       </c>
@@ -8038,8 +9224,11 @@
       <c r="L183" s="1" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="184" spans="1:12" ht="13.2">
+      <c r="M183" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" ht="13.2">
       <c r="A184" s="1" t="s">
         <v>354</v>
       </c>
@@ -8072,8 +9261,11 @@
       <c r="L184" s="1" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="185" spans="1:12" ht="13.2">
+      <c r="M184" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" ht="13.2">
       <c r="A185" s="1" t="s">
         <v>354</v>
       </c>
@@ -8106,8 +9298,11 @@
       <c r="L185" s="1" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="186" spans="1:12" ht="13.2">
+      <c r="M185" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" ht="13.2">
       <c r="A186" s="1" t="s">
         <v>354</v>
       </c>
@@ -8140,8 +9335,11 @@
       <c r="L186" s="1" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="187" spans="1:12" ht="13.2">
+      <c r="M186" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" ht="13.2">
       <c r="A187" s="1" t="s">
         <v>354</v>
       </c>
@@ -8174,8 +9372,11 @@
       <c r="L187" s="1" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="188" spans="1:12" ht="13.2">
+      <c r="M187" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" ht="13.2">
       <c r="A188" s="1" t="s">
         <v>354</v>
       </c>
@@ -8208,8 +9409,11 @@
       <c r="L188" s="1" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="189" spans="1:12" ht="13.2">
+      <c r="M188" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="189" spans="1:13" ht="13.2">
       <c r="A189" s="1" t="s">
         <v>354</v>
       </c>
@@ -8242,8 +9446,11 @@
       <c r="L189" s="1" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="190" spans="1:12" ht="13.2">
+      <c r="M189" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="190" spans="1:13" ht="13.2">
       <c r="A190" s="1" t="s">
         <v>354</v>
       </c>
@@ -8276,8 +9483,11 @@
       <c r="L190" s="1" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="191" spans="1:12" ht="13.2">
+      <c r="M190" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="191" spans="1:13" ht="13.2">
       <c r="A191" s="1" t="s">
         <v>354</v>
       </c>
@@ -8310,8 +9520,11 @@
       <c r="L191" s="1" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="192" spans="1:12" ht="13.2">
+      <c r="M191" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="192" spans="1:13" ht="13.2">
       <c r="A192" s="1" t="s">
         <v>354</v>
       </c>
@@ -8343,8 +9556,11 @@
       <c r="L192" s="1" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="193" spans="1:12" ht="13.2">
+      <c r="M192" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="193" spans="1:13" ht="13.2">
       <c r="A193" s="1" t="s">
         <v>354</v>
       </c>
@@ -8376,8 +9592,11 @@
       <c r="L193" s="1" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="194" spans="1:12" ht="13.2">
+      <c r="M193" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="194" spans="1:13" ht="13.2">
       <c r="A194" s="1" t="s">
         <v>354</v>
       </c>
@@ -8409,8 +9628,11 @@
       <c r="L194" s="1" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="195" spans="1:12" ht="13.2">
+      <c r="M194" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="195" spans="1:13" ht="13.2">
       <c r="A195" s="1" t="s">
         <v>354</v>
       </c>
@@ -8442,8 +9664,11 @@
       <c r="L195" s="1" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="196" spans="1:12" ht="13.2">
+      <c r="M195" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="196" spans="1:13" ht="13.2">
       <c r="A196" s="1" t="s">
         <v>354</v>
       </c>
@@ -8475,8 +9700,11 @@
       <c r="L196" s="1" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="197" spans="1:12" ht="13.2">
+      <c r="M196" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="197" spans="1:13" ht="13.2">
       <c r="A197" s="1" t="s">
         <v>354</v>
       </c>
@@ -8508,8 +9736,11 @@
       <c r="L197" s="1" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="198" spans="1:12" ht="13.2">
+      <c r="M197" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="198" spans="1:13" ht="13.2">
       <c r="A198" s="1" t="s">
         <v>354</v>
       </c>
@@ -8541,8 +9772,11 @@
       <c r="L198" s="1" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="199" spans="1:12" ht="13.2">
+      <c r="M198" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="199" spans="1:13" ht="13.2">
       <c r="A199" s="1" t="s">
         <v>354</v>
       </c>
@@ -8574,8 +9808,11 @@
       <c r="L199" s="1" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="200" spans="1:12" ht="13.2">
+      <c r="M199" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="200" spans="1:13" ht="13.2">
       <c r="A200" s="1" t="s">
         <v>354</v>
       </c>
@@ -8607,8 +9844,11 @@
       <c r="L200" s="1" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="201" spans="1:12" ht="13.2">
+      <c r="M200" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="201" spans="1:13" ht="13.2">
       <c r="A201" s="1" t="s">
         <v>354</v>
       </c>
@@ -8640,8 +9880,11 @@
       <c r="L201" s="1" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="202" spans="1:12" ht="13.2">
+      <c r="M201" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="202" spans="1:13" ht="13.2">
       <c r="A202" s="1" t="s">
         <v>354</v>
       </c>
@@ -8673,8 +9916,11 @@
       <c r="L202" s="1" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="203" spans="1:12" ht="13.2">
+      <c r="M202" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="203" spans="1:13" ht="13.2">
       <c r="A203" s="1" t="s">
         <v>354</v>
       </c>
@@ -8706,8 +9952,11 @@
       <c r="L203" s="1" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="204" spans="1:12" ht="13.2">
+      <c r="M203" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="204" spans="1:13" ht="13.2">
       <c r="A204" s="1" t="s">
         <v>354</v>
       </c>
@@ -8739,8 +9988,11 @@
       <c r="L204" s="1" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="205" spans="1:12" ht="13.2">
+      <c r="M204" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="205" spans="1:13" ht="13.2">
       <c r="A205" s="1" t="s">
         <v>354</v>
       </c>
@@ -8772,8 +10024,11 @@
       <c r="L205" s="1" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="206" spans="1:12" ht="13.2">
+      <c r="M205" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="206" spans="1:13" ht="13.2">
       <c r="A206" s="1" t="s">
         <v>354</v>
       </c>
@@ -8805,8 +10060,11 @@
       <c r="L206" s="1" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="207" spans="1:12" ht="13.2">
+      <c r="M206" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="207" spans="1:13" ht="13.2">
       <c r="A207" s="1" t="s">
         <v>354</v>
       </c>
@@ -8838,8 +10096,11 @@
       <c r="L207" s="1" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="208" spans="1:12" ht="13.2">
+      <c r="M207" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="208" spans="1:13" ht="13.2">
       <c r="A208" s="1" t="s">
         <v>354</v>
       </c>
@@ -8871,8 +10132,11 @@
       <c r="L208" s="1" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="209" spans="1:12" ht="13.2">
+      <c r="M208" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="209" spans="1:13" ht="13.2">
       <c r="A209" s="1" t="s">
         <v>354</v>
       </c>
@@ -8904,8 +10168,11 @@
       <c r="L209" s="1" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="210" spans="1:12" ht="13.2">
+      <c r="M209" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="210" spans="1:13" ht="13.2">
       <c r="A210" s="1" t="s">
         <v>354</v>
       </c>
@@ -8937,8 +10204,11 @@
       <c r="L210" s="1" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="211" spans="1:12" ht="13.2">
+      <c r="M210" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="211" spans="1:13" ht="13.2">
       <c r="A211" s="1" t="s">
         <v>354</v>
       </c>
@@ -8970,8 +10240,11 @@
       <c r="L211" s="1" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="212" spans="1:12" ht="13.2">
+      <c r="M211" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="212" spans="1:13" ht="13.2">
       <c r="A212" s="1" t="s">
         <v>354</v>
       </c>
@@ -9003,8 +10276,11 @@
       <c r="L212" s="1" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="213" spans="1:12" ht="13.2">
+      <c r="M212" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="213" spans="1:13" ht="13.2">
       <c r="A213" s="1" t="s">
         <v>354</v>
       </c>
@@ -9036,8 +10312,11 @@
       <c r="L213" s="1" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="214" spans="1:12" ht="13.2">
+      <c r="M213" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="214" spans="1:13" ht="13.2">
       <c r="A214" s="1" t="s">
         <v>354</v>
       </c>
@@ -9069,8 +10348,11 @@
       <c r="L214" s="1" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="215" spans="1:12" ht="13.2">
+      <c r="M214" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="215" spans="1:13" ht="13.2">
       <c r="A215" s="1" t="s">
         <v>354</v>
       </c>
@@ -9102,40 +10384,43 @@
       <c r="L215" s="1" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="216" spans="1:12" ht="13.2">
+      <c r="M215" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="216" spans="1:13" ht="13.2">
       <c r="F216" s="2"/>
       <c r="J216" s="7"/>
     </row>
-    <row r="217" spans="1:12" ht="13.2">
+    <row r="217" spans="1:13" ht="13.2">
       <c r="F217" s="2"/>
       <c r="J217" s="7"/>
     </row>
-    <row r="218" spans="1:12" ht="13.2">
+    <row r="218" spans="1:13" ht="13.2">
       <c r="F218" s="2"/>
       <c r="J218" s="7"/>
     </row>
-    <row r="219" spans="1:12" ht="13.2">
+    <row r="219" spans="1:13" ht="13.2">
       <c r="F219" s="2"/>
       <c r="J219" s="7"/>
     </row>
-    <row r="220" spans="1:12" ht="13.2">
+    <row r="220" spans="1:13" ht="13.2">
       <c r="F220" s="2"/>
       <c r="J220" s="7"/>
     </row>
-    <row r="221" spans="1:12" ht="13.2">
+    <row r="221" spans="1:13" ht="13.2">
       <c r="F221" s="2"/>
       <c r="J221" s="7"/>
     </row>
-    <row r="222" spans="1:12" ht="13.2">
+    <row r="222" spans="1:13" ht="13.2">
       <c r="F222" s="2"/>
       <c r="J222" s="7"/>
     </row>
-    <row r="223" spans="1:12" ht="13.2">
+    <row r="223" spans="1:13" ht="13.2">
       <c r="F223" s="2"/>
       <c r="J223" s="7"/>
     </row>
-    <row r="224" spans="1:12" ht="13.2">
+    <row r="224" spans="1:13" ht="13.2">
       <c r="F224" s="2"/>
       <c r="J224" s="7"/>
     </row>

</xml_diff>